<commit_message>
quarterly updates TLSA, PLTR
</commit_message>
<xml_diff>
--- a/Automotive/P911.xlsx
+++ b/Automotive/P911.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\models\Automotive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319BD62B-05AB-4DEB-A9B5-35D7D3B346FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2154C5-EF12-495F-AFAA-B24D7F81F0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1035" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -13486,8 +13486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16918,11 +16918,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D37F5735-5460-414D-B5FC-C83DFBD00ECA}">
   <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V4" sqref="V4"/>
+      <selection pane="bottomRight" activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18725,6 +18725,90 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="J14:U14">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15:U19">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15:U15">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16:U16">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17:U17">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J18:U18">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J19:U19">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>